<commit_message>
Begin revising spreadsheet based off new formula
</commit_message>
<xml_diff>
--- a/Probability_of_war/Nuclear war p-values.xlsx
+++ b/Probability_of_war/Nuclear war p-values.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532"/>
   </bookViews>
   <sheets>
-    <sheet name="Upper bound p-values" sheetId="1" r:id="rId1"/>
-    <sheet name="Upper bound forecasting" sheetId="2" r:id="rId2"/>
+    <sheet name="Corrected upper bound p-values" sheetId="3" r:id="rId1"/>
+    <sheet name="Upper bound p-values" sheetId="1" r:id="rId2"/>
+    <sheet name="Upper bound forecasting" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>One in x year odds of nuclear war (alternative hypothesis)</t>
   </si>
@@ -50,12 +51,43 @@
   <si>
     <t>Based on the 2021 upper bound, this is the chance of humanity reaching March 2022 without a nuclear exchange</t>
   </si>
+  <si>
+    <t>CORRECTED BASED ON THE FORMULA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from Global Catastrophic Risk Institute Working Paper 18-1, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A Model For The Probability Of Nuclear War, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seth D. Baum, Robert de Neufville, and Anthony M. Barrett</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +105,23 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,6 +207,790 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5055166" cy="703911"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="525780" y="0"/>
+              <a:ext cx="5055166" cy="703911"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐹</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐴</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑡</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=1− </m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:latin typeface="+mn-lt"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑒</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>−</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝜆</m:t>
+                            </m:r>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="+mn-lt"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑡</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100" i="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>where</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100" b="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝐹</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝐴</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                  <m:d>
+                    <m:dPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:dPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑡</m:t>
+                      </m:r>
+                    </m:e>
+                  </m:d>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>=</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> probability of event A (nuclear war), occuring during a time duration of period t</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝜆</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> = inferred annualized rate of A (A occurs </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <m:rPr>
+                      <m:sty m:val="p"/>
+                    </m:rPr>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>on</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t> </m:t>
+                  </m:r>
+                  <m:r>
+                    <m:rPr>
+                      <m:sty m:val="p"/>
+                    </m:rPr>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>average</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t> </m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝜆</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> times per year)</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="525780" y="0"/>
+              <a:ext cx="5055166" cy="703911"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐹_𝐴 (𝑡)=1− 𝑒^(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>−𝜆𝑡</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" i="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>where</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" b="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐹_𝐴 (𝑡)=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> probability of event A (nuclear war), occuring during a time duration of period t</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜆</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> = inferred annualized rate of A (A occurs </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>on average </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝜆</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> times per year)</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,13 +1256,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>EXP(1)</f>
+        <v>2.7182818284590451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FM359"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10325,7 +11191,7 @@
         <v>2054</v>
       </c>
       <c r="C115">
-        <f t="shared" ref="C115:C146" si="55">(1-C$4)^(B115-1945.75)</f>
+        <f t="shared" ref="C115:C131" si="55">(1-C$4)^(B115-1945.75)</f>
         <v>1.3736631274339082E-2</v>
       </c>
       <c r="D115">
@@ -16526,11 +17392,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>

</xml_diff>